<commit_message>
updated delete function for table
</commit_message>
<xml_diff>
--- a/modules/azzubair_family.xlsx
+++ b/modules/azzubair_family.xlsx
@@ -572,7 +572,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AMNAH</t>
+          <t>AZEMAN</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -582,14 +582,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Daughter</t>
+          <t>Son</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AZEMAN</t>
+          <t>AZIZAH</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -599,14 +599,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Son</t>
+          <t>Daughter</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AZIZAH</t>
+          <t>AZIAH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -623,7 +623,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AZIAH</t>
+          <t>AMNAH</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -640,63 +640,63 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AZZUBAIR</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Son</t>
+          <t>Daughter</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AMMAR</t>
+          <t>FUZIAH</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Son</t>
+          <t>Daughter</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IZZAHTI</t>
+          <t>HANAFIAH</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Daughter</t>
+          <t>Son</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>FARID</t>
+          <t>AZAHARI</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -708,46 +708,46 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ARIFF</t>
+          <t>MASTURA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Son</t>
+          <t>Daughter</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IFFAH</t>
+          <t>DZULKARNAIN</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Daughter</t>
+          <t>Son</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AWATIF</t>
+          <t>NORA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KARTINAH</t>
+          <t>HAMZAH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>FUZIAH</t>
+          <t>ARBA'IYAH</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HANAFIAH</t>
+          <t>HAFIZAH</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -786,19 +786,19 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Son</t>
+          <t>Daughter</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AZAHARI</t>
+          <t>AZZUBAIR</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,29 +810,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MASTURA</t>
+          <t>AMMAR</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Daughter</t>
+          <t>Son</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NORA</t>
+          <t>IZZAHTI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -844,12 +844,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DZULKARNAIN</t>
+          <t>FARID</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,29 +861,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>ARIFF</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>KARTINAH</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>HAMZAH</t>
-        </is>
-      </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Daughter</t>
+          <t>Son</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ARBA'IYAH</t>
+          <t>IFFAH</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -895,12 +895,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HAFIZAH</t>
+          <t>AWATIF</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>HAMZAH</t>
+          <t>KARTINAH</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">

</xml_diff>